<commit_message>
Tagesbericht und Pflichtenheft aktualisiert
</commit_message>
<xml_diff>
--- a/Dokumente/Tagesbericht Mittelstufenprojekt (Derksen, Horstmann, Tahta, Moors).xlsx
+++ b/Dokumente/Tagesbericht Mittelstufenprojekt (Derksen, Horstmann, Tahta, Moors).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Ausbildung\Mittelstufenprojekt-Git\Kassensystem\Dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>Tätigkeitsbezeichnung</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Horstmann</t>
+  </si>
+  <si>
+    <t>10.20 Uhr -  12.00 Uhr</t>
   </si>
 </sst>
 </file>
@@ -545,7 +548,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -771,7 +774,7 @@
         <v>35</v>
       </c>
       <c r="E14" s="5">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="F14" t="s">
         <v>33</v>
@@ -805,7 +808,7 @@
         <v>42865</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E16" s="5">
         <v>0.4</v>

</xml_diff>

<commit_message>
Updated: Pflichtenheft und Tgesbericht
</commit_message>
<xml_diff>
--- a/Dokumente/Tagesbericht Mittelstufenprojekt (Derksen, Horstmann, Tahta, Moors).xlsx
+++ b/Dokumente/Tagesbericht Mittelstufenprojekt (Derksen, Horstmann, Tahta, Moors).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>Tätigkeitsbezeichnung</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Pflichtenheft bearbeiten</t>
   </si>
   <si>
-    <t>Tahta, Derksen</t>
-  </si>
-  <si>
     <t>In Bearbeitung</t>
   </si>
   <si>
@@ -150,6 +147,33 @@
   </si>
   <si>
     <t>10.20 Uhr -  12.00 Uhr</t>
+  </si>
+  <si>
+    <t>Anwendungsfalldiagramm</t>
+  </si>
+  <si>
+    <t>Fertig</t>
+  </si>
+  <si>
+    <t>9.35 Uhr - 11.00 Uhr</t>
+  </si>
+  <si>
+    <t>Tahta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.10 Uhr - </t>
+  </si>
+  <si>
+    <t>in Bearbeitung</t>
+  </si>
+  <si>
+    <t>Layout Design implementieren</t>
+  </si>
+  <si>
+    <t>Derksen</t>
+  </si>
+  <si>
+    <t>Backend implementieren</t>
   </si>
 </sst>
 </file>
@@ -191,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -203,6 +227,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -545,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -690,16 +715,25 @@
       <c r="E7" s="5">
         <v>0</v>
       </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
-        <v>16</v>
+      <c r="C8" s="4">
+        <v>42872</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="E8" s="5">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -728,16 +762,34 @@
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="4">
+        <v>42865</v>
+      </c>
       <c r="E11" s="5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="B12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="4">
+        <v>42872</v>
+      </c>
       <c r="E12" s="5">
-        <v>0</v>
+        <v>0.2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -765,27 +817,27 @@
         <v>32</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="6">
         <v>42865</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="5">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="F14" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="4">
         <v>42865</v>
@@ -794,27 +846,87 @@
         <v>0.2</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="C16" s="4">
         <v>42865</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5">
         <v>0.4</v>
       </c>
       <c r="F16" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="4">
+        <v>42872</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="5">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="4">
+        <v>42872</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="4">
+        <v>42872</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>